<commit_message>
adding files and deleting files
</commit_message>
<xml_diff>
--- a/Raw_Data/Butterfly_Data/Location_Data.xlsx
+++ b/Raw_Data/Butterfly_Data/Location_Data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cowboy/Desktop/Final_Project/Monarch_Climate_Project/Raw_Data/Butterfly_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08A00FC2-8C3A-664D-B42F-03FE006DEA89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F7EC3F-25C2-5E47-B3E3-96A7B40A6706}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15420" xr2:uid="{C90C0ADA-D1CD-184D-AC28-2FF46099041E}"/>
+    <workbookView xWindow="920" yWindow="2580" windowWidth="27240" windowHeight="15420" xr2:uid="{C90C0ADA-D1CD-184D-AC28-2FF46099041E}"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Counties</t>
   </si>
@@ -45,164 +45,62 @@
     <t>Latitude</t>
   </si>
   <si>
-    <t>Average. Count Over 20 Years</t>
-  </si>
-  <si>
     <t>Mendocino</t>
   </si>
   <si>
-    <t>123.4384° W</t>
-  </si>
-  <si>
-    <t>39.5500° N</t>
-  </si>
-  <si>
     <t>Sonoma</t>
   </si>
   <si>
-    <t>122.9888° W</t>
-  </si>
-  <si>
-    <t>38.5780° N</t>
-  </si>
-  <si>
     <t>Marin</t>
   </si>
   <si>
-    <t>122.7633° W</t>
-  </si>
-  <si>
-    <t>38.0834° N</t>
-  </si>
-  <si>
     <t>San Francisco</t>
   </si>
   <si>
-    <t>122.4194° W</t>
-  </si>
-  <si>
-    <t>37.7749° N</t>
-  </si>
-  <si>
     <t>Solano</t>
   </si>
   <si>
-    <t>121.9018° W</t>
-  </si>
-  <si>
-    <t>38.3105° N</t>
-  </si>
-  <si>
     <t>Contra Costa</t>
   </si>
   <si>
-    <t>37.8534° N</t>
-  </si>
-  <si>
     <t>Alameda</t>
   </si>
   <si>
-    <t>121.7195° W</t>
-  </si>
-  <si>
-    <t>37.6017° N</t>
-  </si>
-  <si>
     <t>San Mateo</t>
   </si>
   <si>
-    <t>122.4014° W</t>
-  </si>
-  <si>
-    <t>37.4337° N</t>
-  </si>
-  <si>
     <t>Santa Cruz</t>
   </si>
   <si>
-    <t>121.9580° W</t>
-  </si>
-  <si>
-    <t>37.0454° N</t>
-  </si>
-  <si>
     <t>Monterey</t>
   </si>
   <si>
-    <t>121.3542° W</t>
-  </si>
-  <si>
-    <t>36.3136° N</t>
-  </si>
-  <si>
     <t>San Luis Obispo</t>
   </si>
   <si>
-    <t>120.4358° W</t>
-  </si>
-  <si>
-    <t>35.3102° N</t>
-  </si>
-  <si>
     <t>Santa Barbara</t>
   </si>
   <si>
-    <t>119.6982° W</t>
-  </si>
-  <si>
-    <t>34.4208° N</t>
-  </si>
-  <si>
     <t>Ventura</t>
   </si>
   <si>
-    <t>119.1391° W</t>
-  </si>
-  <si>
-    <t>34.3705° N</t>
-  </si>
-  <si>
     <t>Los Angeles</t>
   </si>
   <si>
-    <t>118.2437° W</t>
-  </si>
-  <si>
-    <t>34.0522° N</t>
-  </si>
-  <si>
     <t>Orange</t>
   </si>
   <si>
-    <t>117.8311° W</t>
-  </si>
-  <si>
-    <t>33.7175° N</t>
-  </si>
-  <si>
     <t>San Diego</t>
   </si>
   <si>
-    <t>117.1611° W</t>
-  </si>
-  <si>
-    <t>32.7157° N</t>
-  </si>
-  <si>
     <t>Inyo</t>
-  </si>
-  <si>
-    <t>36.3092° N</t>
-  </si>
-  <si>
-    <t>117.5496° W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -217,11 +115,6 @@
       <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -245,11 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,18 +456,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8846E49-C9AF-2941-B08F-6CDF782DFA9C}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="3" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -585,246 +479,192 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" s="2">
+        <v>-123.4384</v>
+      </c>
+      <c r="C2" s="2">
+        <v>39.549999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2">
+        <v>-122.9888</v>
+      </c>
+      <c r="C3" s="2">
+        <v>38.578000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B4" s="2">
+        <v>-122.7633</v>
+      </c>
+      <c r="C4" s="2">
+        <v>38.083399999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3">
-        <v>0.25396825396825401</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B5" s="2">
+        <v>-122.4194</v>
+      </c>
+      <c r="C5" s="2">
+        <v>37.774900000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B6" s="2">
+        <v>-121.90179999999999</v>
+      </c>
+      <c r="C6" s="2">
+        <v>38.310499999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B7" s="2">
+        <v>-121.90179999999999</v>
+      </c>
+      <c r="C7" s="2">
+        <v>37.853400000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3">
-        <v>66.030952380952385</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+      <c r="B8" s="2">
+        <v>-121.7195</v>
+      </c>
+      <c r="C8" s="2">
+        <v>37.601700000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B9" s="2">
+        <v>-122.4014</v>
+      </c>
+      <c r="C9" s="2">
+        <v>37.433700000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B10" s="2">
+        <v>-121.958</v>
+      </c>
+      <c r="C10" s="2">
+        <v>37.045400000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1">
-        <v>1135.5131872294373</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+      <c r="B11" s="2">
+        <v>-121.35420000000001</v>
+      </c>
+      <c r="C11" s="2">
+        <v>36.313600000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B12" s="2">
+        <v>-120.4358</v>
+      </c>
+      <c r="C12" s="2">
+        <v>35.310200000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="B13" s="2">
+        <v>-119.6982</v>
+      </c>
+      <c r="C13" s="2">
+        <v>34.4208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1">
-        <v>8.4922524565381696</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+      <c r="B14" s="2">
+        <v>-119.1391</v>
+      </c>
+      <c r="C14" s="2">
+        <v>34.3705</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B15" s="2">
+        <v>-118.2437</v>
+      </c>
+      <c r="C15" s="2">
+        <v>34.052199999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="B16" s="2">
+        <v>-117.83110000000001</v>
+      </c>
+      <c r="C16" s="2">
+        <v>33.717500000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="1">
-        <v>12.285714285714286</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+      <c r="B17" s="2">
+        <v>-117.1611</v>
+      </c>
+      <c r="C17" s="2">
+        <v>32.715699999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1">
-        <v>70.11904761904762</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1507.8650793650795</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1.5952380952380953</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2050.0953509453511</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="1">
-        <v>3094.8936049273507</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2287.2379933524462</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2171.7065594734845</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="3">
-        <v>1487.6293547722119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="1">
-        <v>152.59911055331224</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="3">
-        <v>30.059862227719378</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="1">
-        <v>19.460450144009748</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="1">
-        <v>4.2539682539682548</v>
+      <c r="B18" s="2">
+        <v>-117.5496</v>
+      </c>
+      <c r="C18" s="2">
+        <v>36.309199999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>